<commit_message>
🎨 Beginning work on product ranking and colorimetry
</commit_message>
<xml_diff>
--- a/season-4/141-ranking-products/data/augmented-emerald-cup-winners-2022.xlsx
+++ b/season-4/141-ranking-products/data/augmented-emerald-cup-winners-2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="584">
   <si>
     <t>rank</t>
   </si>
@@ -25,12 +25,12 @@
     <t>entry_name</t>
   </si>
   <si>
+    <t>coa_id</t>
+  </si>
+  <si>
     <t>product_name</t>
   </si>
   <si>
-    <t>coa_id</t>
-  </si>
-  <si>
     <t>lab_results_url</t>
   </si>
   <si>
@@ -820,6 +820,249 @@
     <t>Errl Hill – Gazberries</t>
   </si>
   <si>
+    <t xml:space="preserve"> 220303R058-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q051-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220317Q007-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R055-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R046-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220317Q010-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q043-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R076-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220317Q011-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R049-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S049-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R078-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R080-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q056-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q047-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R065-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R056-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q055-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R084-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S008-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R063-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224R011-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R023-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R047-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R072-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R083-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R049-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R044-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S053-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S050-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S052-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224Q057-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S051-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R086-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S052-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S009-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224Q049-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R055-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S046-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S031-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224Q051-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220317Q005-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q029-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S037-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R036-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220304S019-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224Q048-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S057-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224R003-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S054-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R032-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R031-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q027-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224Q070-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224R006-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R029-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R031-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220224Q031-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R100-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q022-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220228R030-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q032-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q036-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q035-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q038-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S061-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R043-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R053-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R029-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220308R053-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220309S042-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220309S014-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R039-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S004-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220303R028-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S023-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q048-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q041-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307R016-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220301Q025-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 220307S025-001</t>
+  </si>
+  <si>
     <t>Lemon Sponge Cake</t>
   </si>
   <si>
@@ -1334,195 +1577,6 @@
   </si>
   <si>
     <t>Gazberries</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220303R058-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q051-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220317Q007-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220228R055-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220228R046-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220317Q010-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R076-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220317Q011-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220228R049-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R078-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R080-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q056-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q047-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220228R056-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R084-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220304S008-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R063-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220224R011-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220303R047-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R072-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R083-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220304S053-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220304S052-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220224Q057-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R086-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307S052-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220304S009-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220224Q049-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220303R055-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220304S046-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220224Q051-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q029-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220304S037-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220228R036-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220224Q048-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307S057-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307S054-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220303R032-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220303R031-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q027-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220224R006-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220228R031-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R100-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q022-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220228R030-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q032-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q036-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q035-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307S061-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R053-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R029-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220308R053-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220309S042-002</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220309S014-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R039-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307S004-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220303R028-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307S023-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q048-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q041-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307R016-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220301Q025-001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 220307S025-001</t>
   </si>
   <si>
     <t>https://client.sclabs.com/verify/220303R058</t>
@@ -2125,10 +2179,10 @@
         <v>268</v>
       </c>
       <c r="F2" t="s">
-        <v>440</v>
+        <v>349</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>503</v>
+        <v>521</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2148,10 +2202,10 @@
         <v>269</v>
       </c>
       <c r="F3" t="s">
-        <v>441</v>
+        <v>350</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>504</v>
+        <v>522</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2171,10 +2225,10 @@
         <v>270</v>
       </c>
       <c r="F4" t="s">
-        <v>442</v>
+        <v>351</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>505</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2194,10 +2248,10 @@
         <v>269</v>
       </c>
       <c r="F5" t="s">
-        <v>441</v>
+        <v>350</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>504</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2217,10 +2271,10 @@
         <v>271</v>
       </c>
       <c r="F6" t="s">
-        <v>443</v>
+        <v>352</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2240,10 +2294,10 @@
         <v>272</v>
       </c>
       <c r="F7" t="s">
-        <v>444</v>
+        <v>353</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>507</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2259,8 +2313,8 @@
       <c r="D8" t="s">
         <v>89</v>
       </c>
-      <c r="E8" t="s">
-        <v>273</v>
+      <c r="F8" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2277,13 +2331,13 @@
         <v>90</v>
       </c>
       <c r="E9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F9" t="s">
-        <v>445</v>
+        <v>355</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>508</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2300,7 +2354,10 @@
         <v>91</v>
       </c>
       <c r="E10" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+      <c r="F10" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2317,13 +2374,13 @@
         <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F11" t="s">
-        <v>446</v>
+        <v>357</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>509</v>
+        <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2340,13 +2397,13 @@
         <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F12" t="s">
-        <v>447</v>
+        <v>358</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>510</v>
+        <v>528</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2363,13 +2420,13 @@
         <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F13" t="s">
-        <v>448</v>
+        <v>359</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2386,7 +2443,10 @@
         <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>279</v>
+        <v>278</v>
+      </c>
+      <c r="F14" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2403,13 +2463,13 @@
         <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F15" t="s">
-        <v>449</v>
+        <v>361</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2426,13 +2486,13 @@
         <v>97</v>
       </c>
       <c r="E16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F16" t="s">
-        <v>450</v>
+        <v>362</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2449,13 +2509,13 @@
         <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F17" t="s">
-        <v>451</v>
+        <v>363</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>514</v>
+        <v>532</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2472,13 +2532,13 @@
         <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F18" t="s">
-        <v>452</v>
+        <v>364</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>515</v>
+        <v>533</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2495,7 +2555,10 @@
         <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>284</v>
+        <v>283</v>
+      </c>
+      <c r="F19" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2512,13 +2575,13 @@
         <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F20" t="s">
-        <v>453</v>
+        <v>366</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>516</v>
+        <v>534</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2535,7 +2598,10 @@
         <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>286</v>
+        <v>285</v>
+      </c>
+      <c r="F21" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2552,13 +2618,13 @@
         <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F22" t="s">
-        <v>454</v>
+        <v>368</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>517</v>
+        <v>535</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2575,13 +2641,13 @@
         <v>104</v>
       </c>
       <c r="E23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F23" t="s">
-        <v>455</v>
+        <v>369</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2598,13 +2664,13 @@
         <v>105</v>
       </c>
       <c r="E24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F24" t="s">
-        <v>456</v>
+        <v>370</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>519</v>
+        <v>537</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2621,13 +2687,13 @@
         <v>106</v>
       </c>
       <c r="E25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F25" t="s">
-        <v>457</v>
+        <v>371</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>520</v>
+        <v>538</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2644,7 +2710,10 @@
         <v>107</v>
       </c>
       <c r="E26" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+      <c r="F26" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2661,13 +2730,13 @@
         <v>108</v>
       </c>
       <c r="E27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F27" t="s">
-        <v>458</v>
+        <v>373</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>521</v>
+        <v>539</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2684,13 +2753,13 @@
         <v>109</v>
       </c>
       <c r="E28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F28" t="s">
-        <v>459</v>
+        <v>374</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>522</v>
+        <v>540</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2707,13 +2776,13 @@
         <v>110</v>
       </c>
       <c r="E29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F29" t="s">
-        <v>460</v>
+        <v>375</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>523</v>
+        <v>541</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2730,7 +2799,10 @@
         <v>111</v>
       </c>
       <c r="E30" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="F30" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2747,7 +2819,10 @@
         <v>112</v>
       </c>
       <c r="E31" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="F31" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2764,13 +2839,13 @@
         <v>113</v>
       </c>
       <c r="E32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F32" t="s">
-        <v>461</v>
+        <v>378</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>524</v>
+        <v>542</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2787,7 +2862,10 @@
         <v>114</v>
       </c>
       <c r="E33" t="s">
-        <v>298</v>
+        <v>297</v>
+      </c>
+      <c r="F33" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -2804,13 +2882,13 @@
         <v>115</v>
       </c>
       <c r="E34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F34" t="s">
-        <v>462</v>
+        <v>380</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>525</v>
+        <v>543</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -2827,13 +2905,13 @@
         <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F35" t="s">
-        <v>463</v>
+        <v>381</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>526</v>
+        <v>544</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2850,7 +2928,10 @@
         <v>117</v>
       </c>
       <c r="E36" t="s">
-        <v>301</v>
+        <v>300</v>
+      </c>
+      <c r="F36" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2867,13 +2948,13 @@
         <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F37" t="s">
-        <v>464</v>
+        <v>383</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>527</v>
+        <v>545</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2890,13 +2971,13 @@
         <v>119</v>
       </c>
       <c r="E38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F38" t="s">
-        <v>465</v>
+        <v>384</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>528</v>
+        <v>546</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2913,13 +2994,13 @@
         <v>120</v>
       </c>
       <c r="E39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F39" t="s">
-        <v>466</v>
+        <v>385</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>529</v>
+        <v>547</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2936,13 +3017,13 @@
         <v>121</v>
       </c>
       <c r="E40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F40" t="s">
-        <v>467</v>
+        <v>386</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>530</v>
+        <v>548</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2959,13 +3040,13 @@
         <v>122</v>
       </c>
       <c r="E41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F41" t="s">
-        <v>468</v>
+        <v>387</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>531</v>
+        <v>549</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2982,13 +3063,13 @@
         <v>123</v>
       </c>
       <c r="E42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F42" t="s">
-        <v>469</v>
+        <v>388</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>532</v>
+        <v>550</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3005,7 +3086,10 @@
         <v>124</v>
       </c>
       <c r="E43" t="s">
-        <v>308</v>
+        <v>307</v>
+      </c>
+      <c r="F43" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -3022,13 +3106,13 @@
         <v>125</v>
       </c>
       <c r="E44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F44" t="s">
-        <v>470</v>
+        <v>390</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>533</v>
+        <v>551</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3045,7 +3129,10 @@
         <v>126</v>
       </c>
       <c r="E45" t="s">
-        <v>310</v>
+        <v>309</v>
+      </c>
+      <c r="F45" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3062,13 +3149,13 @@
         <v>127</v>
       </c>
       <c r="E46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F46" t="s">
-        <v>471</v>
+        <v>392</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>534</v>
+        <v>552</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3085,13 +3172,13 @@
         <v>128</v>
       </c>
       <c r="E47" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F47" t="s">
-        <v>445</v>
+        <v>355</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>508</v>
+        <v>526</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3108,13 +3195,13 @@
         <v>129</v>
       </c>
       <c r="E48" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F48" t="s">
-        <v>472</v>
+        <v>393</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>535</v>
+        <v>553</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3131,13 +3218,13 @@
         <v>130</v>
       </c>
       <c r="E49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F49" t="s">
-        <v>473</v>
+        <v>394</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>536</v>
+        <v>554</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3154,7 +3241,10 @@
         <v>131</v>
       </c>
       <c r="E50" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="F50" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3171,13 +3261,13 @@
         <v>132</v>
       </c>
       <c r="E51" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F51" t="s">
-        <v>474</v>
+        <v>396</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>537</v>
+        <v>555</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3194,13 +3284,13 @@
         <v>133</v>
       </c>
       <c r="E52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F52" t="s">
-        <v>475</v>
+        <v>397</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>538</v>
+        <v>556</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -3217,7 +3307,10 @@
         <v>134</v>
       </c>
       <c r="E53" t="s">
-        <v>317</v>
+        <v>316</v>
+      </c>
+      <c r="F53" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -3234,13 +3327,13 @@
         <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F54" t="s">
-        <v>460</v>
+        <v>375</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>523</v>
+        <v>541</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3257,13 +3350,13 @@
         <v>136</v>
       </c>
       <c r="E55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F55" t="s">
-        <v>476</v>
+        <v>399</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>539</v>
+        <v>557</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3280,13 +3373,13 @@
         <v>137</v>
       </c>
       <c r="E56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F56" t="s">
-        <v>477</v>
+        <v>400</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>540</v>
+        <v>558</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3303,13 +3396,13 @@
         <v>138</v>
       </c>
       <c r="E57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F57" t="s">
-        <v>478</v>
+        <v>401</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>541</v>
+        <v>559</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -3326,13 +3419,13 @@
         <v>139</v>
       </c>
       <c r="E58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F58" t="s">
-        <v>479</v>
+        <v>402</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>542</v>
+        <v>560</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3349,7 +3442,10 @@
         <v>140</v>
       </c>
       <c r="E59" t="s">
-        <v>322</v>
+        <v>321</v>
+      </c>
+      <c r="F59" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3366,13 +3462,13 @@
         <v>141</v>
       </c>
       <c r="E60" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F60" t="s">
-        <v>480</v>
+        <v>404</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>543</v>
+        <v>561</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3389,7 +3485,10 @@
         <v>142</v>
       </c>
       <c r="E61" t="s">
-        <v>324</v>
+        <v>323</v>
+      </c>
+      <c r="F61" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3406,13 +3505,13 @@
         <v>143</v>
       </c>
       <c r="E62" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F62" t="s">
-        <v>481</v>
+        <v>406</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>544</v>
+        <v>562</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3429,6 +3528,9 @@
         <v>144</v>
       </c>
       <c r="E63" t="s">
+        <v>325</v>
+      </c>
+      <c r="F63" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3449,10 +3551,10 @@
         <v>326</v>
       </c>
       <c r="F64" t="s">
-        <v>482</v>
+        <v>407</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>545</v>
+        <v>563</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3472,10 +3574,10 @@
         <v>327</v>
       </c>
       <c r="F65" t="s">
-        <v>483</v>
+        <v>408</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>546</v>
+        <v>564</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3495,10 +3597,10 @@
         <v>328</v>
       </c>
       <c r="F66" t="s">
-        <v>484</v>
+        <v>409</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3518,10 +3620,10 @@
         <v>329</v>
       </c>
       <c r="F67" t="s">
-        <v>485</v>
+        <v>410</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>548</v>
+        <v>566</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3541,10 +3643,10 @@
         <v>330</v>
       </c>
       <c r="F68" t="s">
-        <v>486</v>
+        <v>411</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3564,10 +3666,10 @@
         <v>331</v>
       </c>
       <c r="F69" t="s">
-        <v>487</v>
+        <v>412</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>550</v>
+        <v>568</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -3586,6 +3688,9 @@
       <c r="E70" t="s">
         <v>332</v>
       </c>
+      <c r="F70" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1">
@@ -3604,10 +3709,10 @@
         <v>333</v>
       </c>
       <c r="F71" t="s">
-        <v>488</v>
+        <v>414</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3626,6 +3731,9 @@
       <c r="E72" t="s">
         <v>334</v>
       </c>
+      <c r="F72" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="1">
@@ -3644,10 +3752,10 @@
         <v>335</v>
       </c>
       <c r="F73" t="s">
-        <v>489</v>
+        <v>416</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>552</v>
+        <v>570</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3663,8 +3771,8 @@
       <c r="D74" t="s">
         <v>155</v>
       </c>
-      <c r="E74" t="s">
-        <v>336</v>
+      <c r="F74" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3680,8 +3788,8 @@
       <c r="D75" t="s">
         <v>156</v>
       </c>
-      <c r="E75" t="s">
-        <v>337</v>
+      <c r="F75" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3698,13 +3806,13 @@
         <v>157</v>
       </c>
       <c r="E76" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F76" t="s">
-        <v>490</v>
+        <v>419</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>553</v>
+        <v>571</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3720,8 +3828,8 @@
       <c r="D77" t="s">
         <v>158</v>
       </c>
-      <c r="E77" t="s">
-        <v>339</v>
+      <c r="F77" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3737,8 +3845,8 @@
       <c r="D78" t="s">
         <v>159</v>
       </c>
-      <c r="E78" t="s">
-        <v>340</v>
+      <c r="F78" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3754,8 +3862,8 @@
       <c r="D79" t="s">
         <v>160</v>
       </c>
-      <c r="E79" t="s">
-        <v>341</v>
+      <c r="F79" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3771,8 +3879,8 @@
       <c r="D80" t="s">
         <v>161</v>
       </c>
-      <c r="E80" t="s">
-        <v>342</v>
+      <c r="F80" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3788,8 +3896,8 @@
       <c r="D81" t="s">
         <v>162</v>
       </c>
-      <c r="E81" t="s">
-        <v>343</v>
+      <c r="F81" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3805,8 +3913,8 @@
       <c r="D82" t="s">
         <v>163</v>
       </c>
-      <c r="E82" t="s">
-        <v>344</v>
+      <c r="F82" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3822,8 +3930,8 @@
       <c r="D83" t="s">
         <v>164</v>
       </c>
-      <c r="E83" t="s">
-        <v>345</v>
+      <c r="F83" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3840,13 +3948,13 @@
         <v>165</v>
       </c>
       <c r="E84" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="F84" t="s">
-        <v>491</v>
+        <v>427</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>554</v>
+        <v>572</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -3863,13 +3971,13 @@
         <v>166</v>
       </c>
       <c r="E85" t="s">
-        <v>347</v>
+        <v>282</v>
       </c>
       <c r="F85" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>515</v>
+        <v>533</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -3885,8 +3993,8 @@
       <c r="D86" t="s">
         <v>167</v>
       </c>
-      <c r="E86" t="s">
-        <v>348</v>
+      <c r="F86" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -3903,13 +4011,13 @@
         <v>168</v>
       </c>
       <c r="E87" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="F87" t="s">
-        <v>492</v>
+        <v>430</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>555</v>
+        <v>573</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -3925,8 +4033,8 @@
       <c r="D88" t="s">
         <v>169</v>
       </c>
-      <c r="E88" t="s">
-        <v>350</v>
+      <c r="F88" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -3943,13 +4051,13 @@
         <v>170</v>
       </c>
       <c r="E89" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F89" t="s">
-        <v>493</v>
+        <v>432</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>556</v>
+        <v>574</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -3965,8 +4073,8 @@
       <c r="D90" t="s">
         <v>171</v>
       </c>
-      <c r="E90" t="s">
-        <v>352</v>
+      <c r="F90" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -3983,13 +4091,13 @@
         <v>172</v>
       </c>
       <c r="E91" t="s">
+        <v>340</v>
+      </c>
+      <c r="F91" t="s">
         <v>38</v>
       </c>
-      <c r="F91" t="s">
-        <v>494</v>
-      </c>
       <c r="G91" s="2" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -4005,8 +4113,8 @@
       <c r="D92" t="s">
         <v>173</v>
       </c>
-      <c r="E92" t="s">
-        <v>353</v>
+      <c r="F92" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4022,8 +4130,8 @@
       <c r="D93" t="s">
         <v>174</v>
       </c>
-      <c r="E93" t="s">
-        <v>354</v>
+      <c r="F93" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4039,8 +4147,8 @@
       <c r="D94" t="s">
         <v>175</v>
       </c>
-      <c r="E94" t="s">
-        <v>355</v>
+      <c r="F94" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -4056,8 +4164,8 @@
       <c r="D95" t="s">
         <v>176</v>
       </c>
-      <c r="E95" t="s">
-        <v>356</v>
+      <c r="F95" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -4073,11 +4181,11 @@
       <c r="D96" t="s">
         <v>177</v>
       </c>
-      <c r="E96" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4090,11 +4198,11 @@
       <c r="D97" t="s">
         <v>178</v>
       </c>
-      <c r="E97" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4107,11 +4215,11 @@
       <c r="D98" t="s">
         <v>179</v>
       </c>
-      <c r="E98" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4124,11 +4232,11 @@
       <c r="D99" t="s">
         <v>180</v>
       </c>
-      <c r="E99" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4141,11 +4249,11 @@
       <c r="D100" t="s">
         <v>181</v>
       </c>
-      <c r="E100" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4158,11 +4266,11 @@
       <c r="D101" t="s">
         <v>182</v>
       </c>
-      <c r="E101" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4175,11 +4283,11 @@
       <c r="D102" t="s">
         <v>183</v>
       </c>
-      <c r="E102" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4192,11 +4300,11 @@
       <c r="D103" t="s">
         <v>184</v>
       </c>
-      <c r="E103" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4209,11 +4317,11 @@
       <c r="D104" t="s">
         <v>185</v>
       </c>
-      <c r="E104" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4226,11 +4334,11 @@
       <c r="D105" t="s">
         <v>186</v>
       </c>
-      <c r="E105" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4243,11 +4351,11 @@
       <c r="D106" t="s">
         <v>187</v>
       </c>
-      <c r="E106" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4260,11 +4368,11 @@
       <c r="D107" t="s">
         <v>188</v>
       </c>
-      <c r="E107" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4277,11 +4385,11 @@
       <c r="D108" t="s">
         <v>189</v>
       </c>
-      <c r="E108" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4294,11 +4402,11 @@
       <c r="D109" t="s">
         <v>190</v>
       </c>
-      <c r="E109" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4311,11 +4419,11 @@
       <c r="D110" t="s">
         <v>191</v>
       </c>
-      <c r="E110" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -4328,11 +4436,11 @@
       <c r="D111" t="s">
         <v>192</v>
       </c>
-      <c r="E111" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -4345,8 +4453,8 @@
       <c r="D112" t="s">
         <v>193</v>
       </c>
-      <c r="E112" t="s">
-        <v>373</v>
+      <c r="F112" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -4362,8 +4470,8 @@
       <c r="D113" t="s">
         <v>194</v>
       </c>
-      <c r="E113" t="s">
-        <v>374</v>
+      <c r="F113" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -4379,8 +4487,8 @@
       <c r="D114" t="s">
         <v>195</v>
       </c>
-      <c r="E114" t="s">
-        <v>375</v>
+      <c r="F114" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -4396,8 +4504,8 @@
       <c r="D115" t="s">
         <v>196</v>
       </c>
-      <c r="E115" t="s">
-        <v>376</v>
+      <c r="F115" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -4413,8 +4521,8 @@
       <c r="D116" t="s">
         <v>197</v>
       </c>
-      <c r="E116" t="s">
-        <v>377</v>
+      <c r="F116" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -4430,8 +4538,8 @@
       <c r="D117" t="s">
         <v>198</v>
       </c>
-      <c r="E117" t="s">
-        <v>378</v>
+      <c r="F117" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -4447,8 +4555,8 @@
       <c r="D118" t="s">
         <v>199</v>
       </c>
-      <c r="E118" t="s">
-        <v>379</v>
+      <c r="F118" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -4464,8 +4572,8 @@
       <c r="D119" t="s">
         <v>200</v>
       </c>
-      <c r="E119" t="s">
-        <v>380</v>
+      <c r="F119" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -4481,8 +4589,8 @@
       <c r="D120" t="s">
         <v>201</v>
       </c>
-      <c r="E120" t="s">
-        <v>381</v>
+      <c r="F120" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -4498,8 +4606,8 @@
       <c r="D121" t="s">
         <v>202</v>
       </c>
-      <c r="E121" t="s">
-        <v>382</v>
+      <c r="F121" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -4516,13 +4624,13 @@
         <v>203</v>
       </c>
       <c r="E122" t="s">
-        <v>383</v>
+        <v>341</v>
       </c>
       <c r="F122" t="s">
-        <v>495</v>
+        <v>464</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4538,8 +4646,8 @@
       <c r="D123" t="s">
         <v>204</v>
       </c>
-      <c r="E123" t="s">
-        <v>384</v>
+      <c r="F123" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -4556,13 +4664,13 @@
         <v>205</v>
       </c>
       <c r="E124" t="s">
-        <v>385</v>
+        <v>342</v>
       </c>
       <c r="F124" t="s">
-        <v>496</v>
+        <v>466</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>559</v>
+        <v>577</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4578,8 +4686,8 @@
       <c r="D125" t="s">
         <v>206</v>
       </c>
-      <c r="E125" t="s">
-        <v>386</v>
+      <c r="F125" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4595,8 +4703,8 @@
       <c r="D126" t="s">
         <v>207</v>
       </c>
-      <c r="E126" t="s">
-        <v>387</v>
+      <c r="F126" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -4612,8 +4720,8 @@
       <c r="D127" t="s">
         <v>208</v>
       </c>
-      <c r="E127" t="s">
-        <v>388</v>
+      <c r="F127" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -4630,16 +4738,16 @@
         <v>209</v>
       </c>
       <c r="E128" t="s">
-        <v>389</v>
+        <v>343</v>
       </c>
       <c r="F128" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4652,11 +4760,11 @@
       <c r="D129" t="s">
         <v>210</v>
       </c>
-      <c r="E129" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4669,11 +4777,11 @@
       <c r="D130" t="s">
         <v>211</v>
       </c>
-      <c r="E130" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4686,11 +4794,11 @@
       <c r="D131" t="s">
         <v>212</v>
       </c>
-      <c r="E131" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4703,11 +4811,11 @@
       <c r="D132" t="s">
         <v>213</v>
       </c>
-      <c r="E132" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4720,11 +4828,11 @@
       <c r="D133" t="s">
         <v>214</v>
       </c>
-      <c r="E133" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4737,11 +4845,11 @@
       <c r="D134" t="s">
         <v>215</v>
       </c>
-      <c r="E134" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4754,11 +4862,11 @@
       <c r="D135" t="s">
         <v>216</v>
       </c>
-      <c r="E135" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4771,11 +4879,11 @@
       <c r="D136" t="s">
         <v>217</v>
       </c>
-      <c r="E136" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4788,11 +4896,11 @@
       <c r="D137" t="s">
         <v>218</v>
       </c>
-      <c r="E137" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4805,11 +4913,11 @@
       <c r="D138" t="s">
         <v>219</v>
       </c>
-      <c r="E138" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4822,11 +4930,11 @@
       <c r="D139" t="s">
         <v>220</v>
       </c>
-      <c r="E139" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4839,11 +4947,11 @@
       <c r="D140" t="s">
         <v>221</v>
       </c>
-      <c r="E140" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4856,11 +4964,11 @@
       <c r="D141" t="s">
         <v>222</v>
       </c>
-      <c r="E141" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4873,11 +4981,11 @@
       <c r="D142" t="s">
         <v>223</v>
       </c>
-      <c r="E142" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4890,11 +4998,11 @@
       <c r="D143" t="s">
         <v>224</v>
       </c>
-      <c r="E143" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4907,11 +5015,11 @@
       <c r="D144" t="s">
         <v>225</v>
       </c>
-      <c r="E144" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4924,11 +5032,11 @@
       <c r="D145" t="s">
         <v>226</v>
       </c>
-      <c r="E145" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4941,11 +5049,11 @@
       <c r="D146" t="s">
         <v>227</v>
       </c>
-      <c r="E146" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4958,11 +5066,11 @@
       <c r="D147" t="s">
         <v>228</v>
       </c>
-      <c r="E147" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4975,11 +5083,11 @@
       <c r="D148" t="s">
         <v>229</v>
       </c>
-      <c r="E148" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
+      <c r="F148" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4992,11 +5100,11 @@
       <c r="D149" t="s">
         <v>230</v>
       </c>
-      <c r="E149" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="F149" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -5009,11 +5117,11 @@
       <c r="D150" t="s">
         <v>231</v>
       </c>
-      <c r="E150" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="F150" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5026,11 +5134,11 @@
       <c r="D151" t="s">
         <v>232</v>
       </c>
-      <c r="E151" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="F151" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5043,11 +5151,11 @@
       <c r="D152" t="s">
         <v>233</v>
       </c>
-      <c r="E152" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="F152" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5060,11 +5168,11 @@
       <c r="D153" t="s">
         <v>234</v>
       </c>
-      <c r="E153" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5077,11 +5185,11 @@
       <c r="D154" t="s">
         <v>232</v>
       </c>
-      <c r="E154" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -5094,11 +5202,11 @@
       <c r="D155" t="s">
         <v>235</v>
       </c>
-      <c r="E155" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="F155" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -5111,11 +5219,11 @@
       <c r="D156" t="s">
         <v>236</v>
       </c>
-      <c r="E156" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -5128,11 +5236,11 @@
       <c r="D157" t="s">
         <v>237</v>
       </c>
-      <c r="E157" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="F157" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -5145,11 +5253,11 @@
       <c r="D158" t="s">
         <v>238</v>
       </c>
-      <c r="E158" t="s">
+      <c r="F158" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:6">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -5162,11 +5270,11 @@
       <c r="D159" t="s">
         <v>239</v>
       </c>
-      <c r="E159" t="s">
+      <c r="F159" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:6">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -5179,11 +5287,11 @@
       <c r="D160" t="s">
         <v>240</v>
       </c>
-      <c r="E160" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5">
+      <c r="F160" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -5196,11 +5304,11 @@
       <c r="D161" t="s">
         <v>241</v>
       </c>
-      <c r="E161" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5">
+      <c r="F161" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -5213,11 +5321,11 @@
       <c r="D162" t="s">
         <v>242</v>
       </c>
-      <c r="E162" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5">
+      <c r="F162" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -5230,11 +5338,11 @@
       <c r="D163" t="s">
         <v>243</v>
       </c>
-      <c r="E163" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5">
+      <c r="F163" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -5247,11 +5355,11 @@
       <c r="D164" t="s">
         <v>244</v>
       </c>
-      <c r="E164" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5">
+      <c r="F164" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -5264,11 +5372,11 @@
       <c r="D165" t="s">
         <v>245</v>
       </c>
-      <c r="E165" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5">
+      <c r="F165" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -5281,11 +5389,11 @@
       <c r="D166" t="s">
         <v>246</v>
       </c>
-      <c r="E166" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5">
+      <c r="F166" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -5298,11 +5406,11 @@
       <c r="D167" t="s">
         <v>247</v>
       </c>
-      <c r="E167" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5">
+      <c r="F167" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -5315,11 +5423,11 @@
       <c r="D168" t="s">
         <v>248</v>
       </c>
-      <c r="E168" t="s">
+      <c r="F168" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:6">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -5332,11 +5440,11 @@
       <c r="D169" t="s">
         <v>249</v>
       </c>
-      <c r="E169" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5">
+      <c r="F169" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -5349,11 +5457,11 @@
       <c r="D170" t="s">
         <v>250</v>
       </c>
-      <c r="E170" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5">
+      <c r="F170" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -5366,11 +5474,11 @@
       <c r="D171" t="s">
         <v>251</v>
       </c>
-      <c r="E171" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5">
+      <c r="F171" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -5383,11 +5491,11 @@
       <c r="D172" t="s">
         <v>252</v>
       </c>
-      <c r="E172" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5">
+      <c r="F172" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -5400,11 +5508,11 @@
       <c r="D173" t="s">
         <v>253</v>
       </c>
-      <c r="E173" t="s">
+      <c r="F173" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:6">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -5417,11 +5525,11 @@
       <c r="D174" t="s">
         <v>254</v>
       </c>
-      <c r="E174" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5">
+      <c r="F174" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -5434,11 +5542,11 @@
       <c r="D175" t="s">
         <v>255</v>
       </c>
-      <c r="E175" t="s">
+      <c r="F175" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:6">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -5451,8 +5559,8 @@
       <c r="D176" t="s">
         <v>256</v>
       </c>
-      <c r="E176" t="s">
-        <v>431</v>
+      <c r="F176" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -5468,8 +5576,8 @@
       <c r="D177" t="s">
         <v>257</v>
       </c>
-      <c r="E177" t="s">
-        <v>432</v>
+      <c r="F177" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -5485,8 +5593,8 @@
       <c r="D178" t="s">
         <v>258</v>
       </c>
-      <c r="E178" t="s">
-        <v>433</v>
+      <c r="F178" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -5502,8 +5610,8 @@
       <c r="D179" t="s">
         <v>259</v>
       </c>
-      <c r="E179" t="s">
-        <v>434</v>
+      <c r="F179" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -5520,13 +5628,13 @@
         <v>260</v>
       </c>
       <c r="E180" t="s">
-        <v>435</v>
+        <v>344</v>
       </c>
       <c r="F180" t="s">
-        <v>498</v>
+        <v>516</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>561</v>
+        <v>579</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -5542,8 +5650,8 @@
       <c r="D181" t="s">
         <v>261</v>
       </c>
-      <c r="E181" t="s">
-        <v>436</v>
+      <c r="F181" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -5560,13 +5668,13 @@
         <v>262</v>
       </c>
       <c r="E182" t="s">
+        <v>345</v>
+      </c>
+      <c r="F182" t="s">
         <v>262</v>
       </c>
-      <c r="F182" t="s">
-        <v>499</v>
-      </c>
       <c r="G182" s="2" t="s">
-        <v>562</v>
+        <v>580</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -5582,7 +5690,7 @@
       <c r="D183" t="s">
         <v>263</v>
       </c>
-      <c r="E183" t="s">
+      <c r="F183" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5597,13 +5705,13 @@
         <v>122</v>
       </c>
       <c r="E184" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F184" t="s">
-        <v>468</v>
+        <v>387</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>531</v>
+        <v>549</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -5620,10 +5728,10 @@
         <v>329</v>
       </c>
       <c r="F185" t="s">
-        <v>485</v>
+        <v>410</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>548</v>
+        <v>566</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -5637,13 +5745,13 @@
         <v>265</v>
       </c>
       <c r="E186" t="s">
-        <v>437</v>
+        <v>346</v>
       </c>
       <c r="F186" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>563</v>
+        <v>581</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -5657,13 +5765,13 @@
         <v>266</v>
       </c>
       <c r="E187" t="s">
-        <v>438</v>
+        <v>347</v>
       </c>
       <c r="F187" t="s">
-        <v>501</v>
+        <v>519</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>564</v>
+        <v>582</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -5677,13 +5785,13 @@
         <v>267</v>
       </c>
       <c r="E188" t="s">
-        <v>439</v>
+        <v>348</v>
       </c>
       <c r="F188" t="s">
-        <v>502</v>
+        <v>520</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>565</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>